<commit_message>
Testing on Mylyn FeatureTool
</commit_message>
<xml_diff>
--- a/RecreationExperiment/Test Results/TestResults.xlsx
+++ b/RecreationExperiment/Test Results/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jen Lee\Desktop\Horizontal-Traceability-Recreaction\RecreationExperiment\Test Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE371E9-9A54-430D-8081-9E3CD0CC925E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347D1519-4BD9-44B5-B7B5-4657B033B007}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18310" windowHeight="9290" activeTab="2" xr2:uid="{2417A0E1-6959-43F0-AE2C-012DA191986F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18310" windowHeight="9290" activeTab="1" xr2:uid="{2417A0E1-6959-43F0-AE2C-012DA191986F}"/>
   </bookViews>
   <sheets>
     <sheet name="ArgoUML" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="64">
   <si>
     <t>ArgoUML</t>
   </si>
@@ -233,12 +233,15 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>(Jen Lee)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +273,12 @@
       <b/>
       <sz val="15"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -535,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -588,9 +597,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -599,6 +605,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -611,6 +620,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -977,10 +992,10 @@
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
@@ -990,10 +1005,10 @@
       <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
+      <c r="I3" s="21"/>
       <c r="J3" s="8" t="s">
         <v>4</v>
       </c>
@@ -1001,37 +1016,37 @@
       <c r="M3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="18"/>
+      <c r="O3" s="21"/>
       <c r="P3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="G4" s="19" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="G4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
-      <c r="M4" s="19" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="20"/>
+      <c r="M4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="20"/>
     </row>
     <row r="5" spans="1:17" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -1151,27 +1166,27 @@
       <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="G8" s="19" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="G8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
-      <c r="M8" s="19" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+      <c r="M8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="21"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="20"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
@@ -1348,10 +1363,10 @@
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="8" t="s">
         <v>4</v>
       </c>
@@ -1359,10 +1374,10 @@
       <c r="G14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="8" t="s">
         <v>4</v>
       </c>
@@ -1370,37 +1385,37 @@
       <c r="M14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N14" s="18" t="s">
+      <c r="N14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="O14" s="18"/>
+      <c r="O14" s="21"/>
       <c r="P14" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="G15" s="19" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="G15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="21"/>
-      <c r="M15" s="19" t="s">
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
+      <c r="M15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="21"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="20"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
@@ -1508,27 +1523,27 @@
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="G19" s="19" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="G19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
-      <c r="M19" s="19" t="s">
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
+      <c r="M19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="21"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
@@ -1687,10 +1702,10 @@
       <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1698,10 +1713,10 @@
       <c r="G25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1709,37 +1724,37 @@
       <c r="M25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N25" s="18" t="s">
+      <c r="N25" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="O25" s="18"/>
+      <c r="O25" s="21"/>
       <c r="P25" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="G26" s="19" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="G26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
-      <c r="M26" s="19" t="s">
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
+      <c r="M26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="21"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="20"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
@@ -1847,27 +1862,27 @@
       <c r="Q29" s="11"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="G30" s="19" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20"/>
+      <c r="G30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="21"/>
-      <c r="M30" s="19" t="s">
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="20"/>
+      <c r="M30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="21"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="20"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
@@ -2026,10 +2041,10 @@
       <c r="A36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="18"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="8" t="s">
         <v>4</v>
       </c>
@@ -2037,10 +2052,10 @@
       <c r="G36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="18"/>
+      <c r="I36" s="21"/>
       <c r="J36" s="8" t="s">
         <v>4</v>
       </c>
@@ -2048,37 +2063,37 @@
       <c r="M36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N36" s="18" t="s">
+      <c r="N36" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="O36" s="18"/>
+      <c r="O36" s="21"/>
       <c r="P36" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
-      <c r="G37" s="19" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="G37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="21"/>
-      <c r="M37" s="19" t="s">
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="20"/>
+      <c r="M37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="21"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="20"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
@@ -2186,27 +2201,27 @@
       <c r="Q40" s="11"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-      <c r="G41" s="19" t="s">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+      <c r="G41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="21"/>
-      <c r="M41" s="19" t="s">
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="20"/>
+      <c r="M41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="21"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="20"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
@@ -2365,10 +2380,10 @@
       <c r="A47" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="18"/>
+      <c r="C47" s="21"/>
       <c r="D47" s="8" t="s">
         <v>4</v>
       </c>
@@ -2376,30 +2391,30 @@
       <c r="G47" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I47" s="18"/>
+      <c r="I47" s="21"/>
       <c r="J47" s="8" t="s">
         <v>4</v>
       </c>
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21"/>
-      <c r="G48" s="19" t="s">
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20"/>
+      <c r="G48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="21"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="20"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
@@ -2474,20 +2489,20 @@
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
-      <c r="G52" s="19" t="s">
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="G52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="21"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="20"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
@@ -2597,18 +2612,20 @@
     <row r="80" ht="25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="M41:Q41"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="G48:K48"/>
+    <mergeCell ref="G52:K52"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="M26:Q26"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="M37:Q37"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="M4:Q4"/>
     <mergeCell ref="M8:Q8"/>
@@ -2621,25 +2638,23 @@
     <mergeCell ref="M19:Q19"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G8:K8"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="G26:K26"/>
     <mergeCell ref="G30:K30"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="M26:Q26"/>
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="G37:K37"/>
     <mergeCell ref="G41:K41"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="M37:Q37"/>
-    <mergeCell ref="M41:Q41"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="G48:K48"/>
-    <mergeCell ref="G52:K52"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2650,8 +2665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1896567F-D6D5-45A1-B7A7-42A7EF5D174A}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2699,10 +2714,10 @@
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
@@ -2712,48 +2727,52 @@
       <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="18"/>
+      <c r="I3" s="21"/>
       <c r="J3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="9"/>
+      <c r="K3" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="18"/>
+      <c r="O3" s="21"/>
       <c r="P3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="9"/>
+      <c r="Q3" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="G4" s="19" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="G4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
-      <c r="M4" s="19" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="20"/>
+      <c r="M4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="20"/>
     </row>
     <row r="5" spans="1:17" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -2861,27 +2880,27 @@
       <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="G8" s="19" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="G8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
-      <c r="M8" s="19" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+      <c r="M8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="21"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="20"/>
     </row>
     <row r="9" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
@@ -2905,22 +2924,30 @@
       <c r="H9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="6">
+        <v>9.3921770000000002E-2</v>
+      </c>
       <c r="J9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="11"/>
+      <c r="K9" s="11">
+        <v>3.1647269999999998E-2</v>
+      </c>
       <c r="M9" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="6"/>
+      <c r="O9" s="6">
+        <v>0.1037448</v>
+      </c>
       <c r="P9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q9" s="11"/>
+      <c r="Q9" s="11">
+        <v>3.0281760000000001E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
@@ -2944,22 +2971,30 @@
       <c r="H10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5">
+        <v>3.8</v>
+      </c>
       <c r="J10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="12"/>
+      <c r="K10" s="12">
+        <v>71.55</v>
+      </c>
       <c r="M10" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="5"/>
+      <c r="O10" s="5">
+        <v>3.33</v>
+      </c>
       <c r="P10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q10" s="12"/>
+      <c r="Q10" s="12">
+        <v>75.12</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
@@ -2983,22 +3018,30 @@
       <c r="H11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5">
+        <v>80</v>
+      </c>
       <c r="J11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="12"/>
+      <c r="K11" s="26">
+        <v>100</v>
+      </c>
       <c r="M11" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="5"/>
+      <c r="O11" s="5">
+        <v>90</v>
+      </c>
       <c r="P11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q11" s="12"/>
+      <c r="Q11" s="12">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
@@ -3054,63 +3097,69 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="G14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="9"/>
+      <c r="K14" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N14" s="18" t="s">
+      <c r="N14" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="O14" s="18"/>
+      <c r="O14" s="21"/>
       <c r="P14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q14" s="9"/>
+      <c r="Q14" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="G15" s="19" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="G15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="21"/>
-      <c r="M15" s="19" t="s">
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
+      <c r="M15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="21"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="20"/>
     </row>
     <row r="16" spans="1:17" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
@@ -3218,132 +3267,168 @@
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="G19" s="19" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="G19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
-      <c r="M19" s="19" t="s">
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
+      <c r="M19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="21"/>
-    </row>
-    <row r="20" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="20"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="6">
+        <v>0.12451230000000001</v>
+      </c>
       <c r="D20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="11"/>
+      <c r="E20" s="11">
+        <v>2.6960660000000001E-2</v>
+      </c>
       <c r="G20" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="6"/>
+      <c r="I20" s="6">
+        <v>0.1291168</v>
+      </c>
       <c r="J20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="11"/>
+      <c r="K20" s="11">
+        <v>3.322539E-2</v>
+      </c>
       <c r="M20" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O20" s="6"/>
+      <c r="O20" s="6">
+        <v>0.1011773</v>
+      </c>
       <c r="P20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q20" s="11"/>
-    </row>
-    <row r="21" spans="1:17" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="Q20" s="11">
+        <v>3.2987160000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>3.31</v>
+      </c>
       <c r="D21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="12">
+        <v>66.760000000000005</v>
+      </c>
       <c r="G21" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="5"/>
+      <c r="I21" s="5">
+        <v>3.67</v>
+      </c>
       <c r="J21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K21" s="12"/>
+      <c r="K21" s="12">
+        <v>71.33</v>
+      </c>
       <c r="M21" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O21" s="5"/>
+      <c r="O21" s="5">
+        <v>3.53</v>
+      </c>
       <c r="P21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q21" s="12"/>
-    </row>
-    <row r="22" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+      <c r="Q21" s="12">
+        <v>72.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5">
+        <v>90</v>
+      </c>
       <c r="D22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="12">
+        <v>100</v>
+      </c>
       <c r="G22" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="5"/>
+      <c r="I22" s="5">
+        <v>90</v>
+      </c>
       <c r="J22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="12"/>
+      <c r="K22" s="12">
+        <v>100</v>
+      </c>
       <c r="M22" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O22" s="5"/>
+      <c r="O22" s="27">
+        <v>80</v>
+      </c>
       <c r="P22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q22" s="12"/>
+      <c r="Q22" s="12">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="14" t="s">
@@ -3393,25 +3478,27 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="G25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="8" t="s">
         <v>4</v>
       </c>
@@ -3419,39 +3506,39 @@
       <c r="M25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N25" s="18" t="s">
+      <c r="N25" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="O25" s="18"/>
+      <c r="O25" s="21"/>
       <c r="P25" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="G26" s="19" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="G26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
-      <c r="M26" s="19" t="s">
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
+      <c r="M26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="21"/>
-    </row>
-    <row r="27" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="20"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>7</v>
       </c>
@@ -3557,27 +3644,27 @@
       <c r="Q29" s="11"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="G30" s="19" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20"/>
+      <c r="G30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="21"/>
-      <c r="M30" s="19" t="s">
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="20"/>
+      <c r="M30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="21"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="20"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
@@ -3586,11 +3673,15 @@
       <c r="B31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="6"/>
+      <c r="C31" s="6">
+        <v>9.7668599999999994E-2</v>
+      </c>
       <c r="D31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="11"/>
+      <c r="E31" s="11">
+        <v>6.8918219999999997E-3</v>
+      </c>
       <c r="G31" s="10" t="s">
         <v>7</v>
       </c>
@@ -3621,11 +3712,15 @@
       <c r="B32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>3.86</v>
+      </c>
       <c r="D32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="12"/>
+      <c r="E32" s="12">
+        <v>32.36</v>
+      </c>
       <c r="G32" s="10" t="s">
         <v>27</v>
       </c>
@@ -3656,11 +3751,15 @@
       <c r="B33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="5"/>
+      <c r="C33" s="5">
+        <v>50</v>
+      </c>
       <c r="D33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="26">
+        <v>80</v>
+      </c>
       <c r="G33" s="13" t="s">
         <v>12</v>
       </c>
@@ -3736,10 +3835,10 @@
       <c r="A36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="18"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="8" t="s">
         <v>4</v>
       </c>
@@ -3747,10 +3846,10 @@
       <c r="G36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I36" s="18"/>
+      <c r="I36" s="21"/>
       <c r="J36" s="8" t="s">
         <v>4</v>
       </c>
@@ -3758,37 +3857,37 @@
       <c r="M36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N36" s="18" t="s">
+      <c r="N36" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="O36" s="18"/>
+      <c r="O36" s="21"/>
       <c r="P36" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
-      <c r="G37" s="19" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="G37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="21"/>
-      <c r="M37" s="19" t="s">
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="20"/>
+      <c r="M37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="21"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="20"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
@@ -3896,27 +3995,27 @@
       <c r="Q40" s="11"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-      <c r="G41" s="19" t="s">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+      <c r="G41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="21"/>
-      <c r="M41" s="19" t="s">
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="20"/>
+      <c r="M41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="21"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="20"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
@@ -4075,10 +4174,10 @@
       <c r="A47" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="18"/>
+      <c r="C47" s="21"/>
       <c r="D47" s="8" t="s">
         <v>4</v>
       </c>
@@ -4086,10 +4185,10 @@
       <c r="G47" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I47" s="18"/>
+      <c r="I47" s="21"/>
       <c r="J47" s="8" t="s">
         <v>4</v>
       </c>
@@ -4097,37 +4196,39 @@
       <c r="M47" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N47" s="18" t="s">
+      <c r="N47" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O47" s="18"/>
+      <c r="O47" s="21"/>
       <c r="P47" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q47" s="9"/>
+      <c r="Q47" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21"/>
-      <c r="G48" s="19" t="s">
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20"/>
+      <c r="G48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="21"/>
-      <c r="M48" s="19" t="s">
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="20"/>
+      <c r="M48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N48" s="20"/>
-      <c r="O48" s="20"/>
-      <c r="P48" s="20"/>
-      <c r="Q48" s="21"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="20"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
@@ -4235,27 +4336,27 @@
       <c r="Q51" s="11"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
-      <c r="G52" s="19" t="s">
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="G52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="21"/>
-      <c r="M52" s="19" t="s">
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="20"/>
+      <c r="M52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N52" s="20"/>
-      <c r="O52" s="20"/>
-      <c r="P52" s="20"/>
-      <c r="Q52" s="21"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="20"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
@@ -4286,11 +4387,15 @@
       <c r="N53" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O53" s="6"/>
+      <c r="O53" s="6">
+        <v>3.0193089999999999E-2</v>
+      </c>
       <c r="P53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q53" s="11"/>
+      <c r="Q53" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
@@ -4321,11 +4426,15 @@
       <c r="N54" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O54" s="5"/>
+      <c r="O54" s="5">
+        <v>3.24</v>
+      </c>
       <c r="P54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q54" s="12"/>
+      <c r="Q54" s="12">
+        <v>31.89</v>
+      </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
@@ -4356,11 +4465,15 @@
       <c r="N55" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O55" s="5"/>
+      <c r="O55" s="5">
+        <v>40</v>
+      </c>
       <c r="P55" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q55" s="12"/>
+      <c r="Q55" s="12">
+        <v>70</v>
+      </c>
     </row>
     <row r="56" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="14" t="s">
@@ -4411,36 +4524,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="M26:Q26"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="N36:O36"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="N47:O47"/>
     <mergeCell ref="M48:Q48"/>
@@ -4457,8 +4540,39 @@
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="G41:K41"/>
     <mergeCell ref="M41:Q41"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="M26:Q26"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="M4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4466,7 +4580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B085D52C-782B-41CA-ACF5-3119A9AF2B5C}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4509,10 +4623,10 @@
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
@@ -4522,10 +4636,10 @@
       <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="18"/>
+      <c r="I3" s="21"/>
       <c r="J3" s="8" t="s">
         <v>4</v>
       </c>
@@ -4533,37 +4647,37 @@
       <c r="M3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="18"/>
+      <c r="O3" s="21"/>
       <c r="P3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="G4" s="19" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="G4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
-      <c r="M4" s="19" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="20"/>
+      <c r="M4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="20"/>
     </row>
     <row r="5" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -4675,27 +4789,27 @@
       <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="G8" s="19" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="G8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
-      <c r="M8" s="19" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+      <c r="M8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="21"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="20"/>
     </row>
     <row r="9" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
@@ -4866,10 +4980,10 @@
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="8" t="s">
         <v>4</v>
       </c>
@@ -4877,10 +4991,10 @@
       <c r="G14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="8" t="s">
         <v>4</v>
       </c>
@@ -4888,37 +5002,37 @@
       <c r="M14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N14" s="18" t="s">
+      <c r="N14" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="O14" s="18"/>
+      <c r="O14" s="21"/>
       <c r="P14" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="G15" s="19" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="G15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="21"/>
-      <c r="M15" s="19" t="s">
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
+      <c r="M15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="21"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="20"/>
     </row>
     <row r="16" spans="1:17" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
@@ -5026,29 +5140,29 @@
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="G19" s="19" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="G19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
-      <c r="M19" s="19" t="s">
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
+      <c r="M19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="21"/>
-    </row>
-    <row r="20" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="20"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>7</v>
       </c>
@@ -5083,7 +5197,7 @@
       </c>
       <c r="Q20" s="11"/>
     </row>
-    <row r="21" spans="1:17" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
@@ -5118,7 +5232,7 @@
       </c>
       <c r="Q21" s="12"/>
     </row>
-    <row r="22" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>12</v>
       </c>
@@ -5201,14 +5315,14 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="8" t="s">
         <v>4</v>
       </c>
@@ -5216,10 +5330,10 @@
       <c r="G25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="8" t="s">
         <v>4</v>
       </c>
@@ -5227,39 +5341,39 @@
       <c r="M25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N25" s="18" t="s">
+      <c r="N25" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="O25" s="18"/>
+      <c r="O25" s="21"/>
       <c r="P25" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="G26" s="19" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="G26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
-      <c r="M26" s="19" t="s">
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
+      <c r="M26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="21"/>
-    </row>
-    <row r="27" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="20"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>7</v>
       </c>
@@ -5365,27 +5479,27 @@
       <c r="Q29" s="11"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="G30" s="19" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20"/>
+      <c r="G30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="21"/>
-      <c r="M30" s="19" t="s">
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="20"/>
+      <c r="M30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="21"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="20"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
@@ -5544,10 +5658,10 @@
       <c r="A36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="18"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="8" t="s">
         <v>4</v>
       </c>
@@ -5555,10 +5669,10 @@
       <c r="G36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="18"/>
+      <c r="I36" s="21"/>
       <c r="J36" s="8" t="s">
         <v>4</v>
       </c>
@@ -5566,37 +5680,37 @@
       <c r="M36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N36" s="18" t="s">
+      <c r="N36" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="O36" s="18"/>
+      <c r="O36" s="21"/>
       <c r="P36" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
-      <c r="G37" s="19" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="G37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="21"/>
-      <c r="M37" s="19" t="s">
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="20"/>
+      <c r="M37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="21"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="20"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
@@ -5704,27 +5818,27 @@
       <c r="Q40" s="11"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-      <c r="G41" s="19" t="s">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+      <c r="G41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="21"/>
-      <c r="M41" s="19" t="s">
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="20"/>
+      <c r="M41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="21"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="20"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
@@ -5883,10 +5997,10 @@
       <c r="A47" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="18"/>
+      <c r="C47" s="21"/>
       <c r="D47" s="8" t="s">
         <v>4</v>
       </c>
@@ -5894,30 +6008,30 @@
       <c r="G47" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I47" s="18"/>
+      <c r="I47" s="21"/>
       <c r="J47" s="8" t="s">
         <v>4</v>
       </c>
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21"/>
-      <c r="G48" s="19" t="s">
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20"/>
+      <c r="G48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="21"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="20"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
@@ -5992,20 +6106,20 @@
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
-      <c r="G52" s="19" t="s">
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="G52" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="21"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="20"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
@@ -6113,36 +6227,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="M26:Q26"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="M37:Q37"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="G41:K41"/>
-    <mergeCell ref="M41:Q41"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="N36:O36"/>
     <mergeCell ref="A52:E52"/>
     <mergeCell ref="G52:K52"/>
     <mergeCell ref="A1:K1"/>
@@ -6156,6 +6240,36 @@
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="G8:K8"/>
+    <mergeCell ref="M37:Q37"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="G41:K41"/>
+    <mergeCell ref="M41:Q41"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="M26:Q26"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="M4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finishing testing on Mylyn
</commit_message>
<xml_diff>
--- a/RecreationExperiment/Test Results/TestResults.xlsx
+++ b/RecreationExperiment/Test Results/TestResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jen Lee\Desktop\Horizontal-Traceability-Recreaction\RecreationExperiment\Test Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347D1519-4BD9-44B5-B7B5-4657B033B007}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAEDD56-5AE3-461A-8E1B-AD867F23A144}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18310" windowHeight="9290" activeTab="1" xr2:uid="{2417A0E1-6959-43F0-AE2C-012DA191986F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="63">
   <si>
     <t>ArgoUML</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Mylyn_DW</t>
   </si>
   <si>
-    <t>Mylyn_DW_SC_SP_SM_LO</t>
-  </si>
-  <si>
     <t>Mylyn_LO</t>
   </si>
   <si>
@@ -234,14 +231,14 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>(Jen Lee)</t>
+    <t>Mylyn_DW_SC_SY_SM_LO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +276,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -544,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -625,6 +627,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2665,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1896567F-D6D5-45A1-B7A7-42A7EF5D174A}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2735,7 +2746,7 @@
         <v>4</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>1</v>
@@ -2748,7 +2759,7 @@
         <v>4</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -2774,110 +2785,146 @@
       <c r="P4" s="19"/>
       <c r="Q4" s="20"/>
     </row>
-    <row r="5" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6">
+        <v>0.15518109999999999</v>
+      </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="11">
+        <v>3.184389E-2</v>
+      </c>
       <c r="G5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="6">
+        <v>9.3921770000000002E-2</v>
+      </c>
       <c r="J5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="11"/>
+      <c r="K5" s="11">
+        <v>3.1647269999999998E-2</v>
+      </c>
       <c r="M5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="6"/>
+      <c r="O5" s="6">
+        <v>0.1037448</v>
+      </c>
       <c r="P5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="11"/>
-    </row>
-    <row r="6" spans="1:17" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="Q5" s="11">
+        <v>3.0281760000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5">
+        <v>5.83</v>
+      </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="12">
+        <v>183.68</v>
+      </c>
       <c r="G6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="5">
+        <v>7.02</v>
+      </c>
       <c r="J6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="12"/>
+      <c r="K6" s="12">
+        <v>254.84</v>
+      </c>
       <c r="M6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="5"/>
+      <c r="O6" s="5">
+        <v>7.41</v>
+      </c>
       <c r="P6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="12"/>
-    </row>
-    <row r="7" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+      <c r="Q6" s="12">
+        <v>261.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6">
+        <v>90</v>
+      </c>
       <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="11">
+        <v>100</v>
+      </c>
       <c r="G7" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="6">
+        <v>80</v>
+      </c>
       <c r="J7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="11"/>
+      <c r="K7" s="28">
+        <v>90</v>
+      </c>
       <c r="M7" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="6"/>
+      <c r="O7" s="6">
+        <v>90</v>
+      </c>
       <c r="P7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="11"/>
+      <c r="Q7" s="11">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
@@ -3109,7 +3156,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>1</v>
@@ -3122,7 +3169,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="M14" s="7" t="s">
         <v>1</v>
@@ -3135,7 +3182,7 @@
         <v>4</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
@@ -3161,110 +3208,146 @@
       <c r="P15" s="19"/>
       <c r="Q15" s="20"/>
     </row>
-    <row r="16" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="6">
+        <v>0.12451230000000001</v>
+      </c>
       <c r="D16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11">
+        <v>2.6960660000000001E-2</v>
+      </c>
       <c r="G16" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="6">
+        <v>0.1291168</v>
+      </c>
       <c r="J16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="11"/>
+      <c r="K16" s="11">
+        <v>3.322539E-2</v>
+      </c>
       <c r="M16" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O16" s="6"/>
+      <c r="O16" s="6">
+        <v>0.1011773</v>
+      </c>
       <c r="P16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q16" s="11"/>
-    </row>
-    <row r="17" spans="1:17" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="Q16" s="11">
+        <v>3.2987160000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5">
+        <v>7.3</v>
+      </c>
       <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="12">
+        <v>229.99</v>
+      </c>
       <c r="G17" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5">
+        <v>5.71</v>
+      </c>
       <c r="J17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K17" s="12"/>
+      <c r="K17" s="12">
+        <v>187.37</v>
+      </c>
       <c r="M17" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O17" s="5"/>
+      <c r="O17" s="5">
+        <v>8.09</v>
+      </c>
       <c r="P17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q17" s="12"/>
-    </row>
-    <row r="18" spans="1:17" ht="26" x14ac:dyDescent="0.35">
+      <c r="Q17" s="12">
+        <v>375.21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6">
+        <v>90</v>
+      </c>
       <c r="D18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="11"/>
+      <c r="E18" s="11">
+        <v>100</v>
+      </c>
       <c r="G18" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="6">
+        <v>90</v>
+      </c>
       <c r="J18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="11"/>
+      <c r="K18" s="11">
+        <v>100</v>
+      </c>
       <c r="M18" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="6"/>
+      <c r="O18" s="29">
+        <v>90</v>
+      </c>
       <c r="P18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q18" s="11"/>
+      <c r="Q18" s="11">
+        <v>100</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
@@ -3490,30 +3573,34 @@
         <v>4</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>1</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="9"/>
+      <c r="K25" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="M25" s="7" t="s">
         <v>1</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O25" s="21"/>
       <c r="P25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q25" s="9"/>
+      <c r="Q25" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
@@ -3545,33 +3632,45 @@
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="6">
+        <v>9.7668599999999994E-2</v>
+      </c>
       <c r="D27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="11"/>
+      <c r="E27" s="11">
+        <v>6.8918219999999997E-3</v>
+      </c>
       <c r="G27" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="6"/>
+      <c r="I27" s="6">
+        <v>0.15025240000000001</v>
+      </c>
       <c r="J27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="11"/>
+      <c r="K27" s="11">
+        <v>1.6937540000000001E-2</v>
+      </c>
       <c r="M27" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O27" s="6"/>
+      <c r="O27" s="6">
+        <v>0.1212771</v>
+      </c>
       <c r="P27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q27" s="11"/>
+      <c r="Q27" s="11">
+        <v>7.72619E-3</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
@@ -3580,33 +3679,45 @@
       <c r="B28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>4.62</v>
+      </c>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="12">
+        <v>42.31</v>
+      </c>
       <c r="G28" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="5"/>
+      <c r="I28" s="5">
+        <v>4.2300000000000004</v>
+      </c>
       <c r="J28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="12"/>
+      <c r="K28" s="12">
+        <v>30.18</v>
+      </c>
       <c r="M28" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O28" s="5"/>
+      <c r="O28" s="5">
+        <v>4.7699999999999996</v>
+      </c>
       <c r="P28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q28" s="12"/>
+      <c r="Q28" s="12">
+        <v>36.79</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
@@ -3615,33 +3726,45 @@
       <c r="B29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="6">
+        <v>50</v>
+      </c>
       <c r="D29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="11"/>
+      <c r="E29" s="11">
+        <v>70</v>
+      </c>
       <c r="G29" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="6"/>
+      <c r="I29" s="29">
+        <v>50</v>
+      </c>
       <c r="J29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K29" s="11"/>
+      <c r="K29" s="28">
+        <v>80</v>
+      </c>
       <c r="M29" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O29" s="6"/>
+      <c r="O29" s="6">
+        <v>50</v>
+      </c>
       <c r="P29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q29" s="11"/>
+      <c r="Q29" s="11">
+        <v>60</v>
+      </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
@@ -3688,22 +3811,30 @@
       <c r="H31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I31" s="6"/>
+      <c r="I31" s="6">
+        <v>0.15025240000000001</v>
+      </c>
       <c r="J31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K31" s="11"/>
+      <c r="K31" s="11">
+        <v>1.6937540000000001E-2</v>
+      </c>
       <c r="M31" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O31" s="6"/>
+      <c r="O31" s="6">
+        <v>0.1212771</v>
+      </c>
       <c r="P31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q31" s="11"/>
+      <c r="Q31" s="11">
+        <v>7.72619E-3</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
@@ -3727,22 +3858,30 @@
       <c r="H32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I32" s="5"/>
+      <c r="I32" s="5">
+        <v>3.32</v>
+      </c>
       <c r="J32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="12"/>
+      <c r="K32" s="12">
+        <v>33.15</v>
+      </c>
       <c r="M32" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O32" s="5"/>
+      <c r="O32" s="5">
+        <v>2.79</v>
+      </c>
       <c r="P32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q32" s="12"/>
+      <c r="Q32" s="12">
+        <v>31.32</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
@@ -3766,22 +3905,30 @@
       <c r="H33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="5"/>
+      <c r="I33" s="27">
+        <v>50</v>
+      </c>
       <c r="J33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K33" s="12"/>
+      <c r="K33" s="26">
+        <v>80</v>
+      </c>
       <c r="M33" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O33" s="5"/>
+      <c r="O33" s="27">
+        <v>40</v>
+      </c>
       <c r="P33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q33" s="12"/>
+      <c r="Q33" s="26">
+        <v>70</v>
+      </c>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="14" t="s">
@@ -3836,35 +3983,41 @@
         <v>1</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="9"/>
+      <c r="E36" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="G36" s="7" t="s">
         <v>1</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I36" s="21"/>
       <c r="J36" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K36" s="9"/>
+      <c r="K36" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="M36" s="7" t="s">
         <v>1</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O36" s="21"/>
       <c r="P36" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q36" s="9"/>
+      <c r="Q36" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
@@ -3896,33 +4049,45 @@
       <c r="B38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="6"/>
+      <c r="C38" s="6">
+        <v>0.1076133</v>
+      </c>
       <c r="D38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="11"/>
+      <c r="E38" s="11">
+        <v>8.3806660000000002E-3</v>
+      </c>
       <c r="G38" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="6"/>
+      <c r="I38" s="6">
+        <v>0.107457</v>
+      </c>
       <c r="J38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K38" s="11"/>
+      <c r="K38" s="11">
+        <v>8.3871550000000003E-3</v>
+      </c>
       <c r="M38" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O38" s="6"/>
+      <c r="O38" s="6">
+        <v>0.12599260000000001</v>
+      </c>
       <c r="P38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q38" s="11"/>
+      <c r="Q38" s="11">
+        <v>1.069295E-2</v>
+      </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
@@ -3931,33 +4096,45 @@
       <c r="B39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="5">
+        <v>3.47</v>
+      </c>
       <c r="D39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="12"/>
+      <c r="E39" s="12">
+        <v>44.37</v>
+      </c>
       <c r="G39" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I39" s="5"/>
+      <c r="I39" s="5">
+        <v>3.25</v>
+      </c>
       <c r="J39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K39" s="12"/>
+      <c r="K39" s="12">
+        <v>44.05</v>
+      </c>
       <c r="M39" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O39" s="5"/>
+      <c r="O39" s="5">
+        <v>5.07</v>
+      </c>
       <c r="P39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q39" s="12"/>
+      <c r="Q39" s="12">
+        <v>35.74</v>
+      </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
@@ -3966,33 +4143,45 @@
       <c r="B40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="6">
+        <v>50</v>
+      </c>
       <c r="D40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="11"/>
+      <c r="E40" s="11">
+        <v>70</v>
+      </c>
       <c r="G40" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="6"/>
+      <c r="I40" s="6">
+        <v>50</v>
+      </c>
       <c r="J40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="11"/>
+      <c r="K40" s="11">
+        <v>70</v>
+      </c>
       <c r="M40" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O40" s="6"/>
+      <c r="O40" s="6">
+        <v>40</v>
+      </c>
       <c r="P40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q40" s="11"/>
+      <c r="Q40" s="11">
+        <v>70</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
@@ -4024,33 +4213,45 @@
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="6"/>
+      <c r="C42" s="6">
+        <v>0.1076133</v>
+      </c>
       <c r="D42" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="11"/>
+      <c r="E42" s="11">
+        <v>8.3806660000000002E-3</v>
+      </c>
       <c r="G42" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="6"/>
+      <c r="I42" s="6">
+        <v>0.107457</v>
+      </c>
       <c r="J42" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K42" s="11"/>
+      <c r="K42" s="11">
+        <v>8.3871550000000003E-3</v>
+      </c>
       <c r="M42" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O42" s="6"/>
+      <c r="O42" s="6">
+        <v>0.12599260000000001</v>
+      </c>
       <c r="P42" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q42" s="11"/>
+      <c r="Q42" s="11">
+        <v>1.069295E-2</v>
+      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
@@ -4059,33 +4260,45 @@
       <c r="B43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="5"/>
+      <c r="C43" s="5">
+        <v>3.68</v>
+      </c>
       <c r="D43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="12"/>
+      <c r="E43" s="12">
+        <v>35.39</v>
+      </c>
       <c r="G43" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="5"/>
+      <c r="I43" s="5">
+        <v>2.94</v>
+      </c>
       <c r="J43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K43" s="12"/>
+      <c r="K43" s="12">
+        <v>37.86</v>
+      </c>
       <c r="M43" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O43" s="5"/>
+      <c r="O43" s="5">
+        <v>4.79</v>
+      </c>
       <c r="P43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q43" s="12"/>
+      <c r="Q43" s="12">
+        <v>47.2</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
@@ -4094,33 +4307,45 @@
       <c r="B44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="5"/>
+      <c r="C44" s="27">
+        <v>40</v>
+      </c>
       <c r="D44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E44" s="12"/>
+      <c r="E44" s="12">
+        <v>70</v>
+      </c>
       <c r="G44" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I44" s="5"/>
+      <c r="I44" s="27">
+        <v>40</v>
+      </c>
       <c r="J44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K44" s="12"/>
+      <c r="K44" s="30">
+        <v>70</v>
+      </c>
       <c r="M44" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O44" s="5"/>
+      <c r="O44" s="5">
+        <v>40</v>
+      </c>
       <c r="P44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q44" s="12"/>
+      <c r="Q44" s="12">
+        <v>70</v>
+      </c>
     </row>
     <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="14" t="s">
@@ -4175,36 +4400,40 @@
         <v>1</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="9"/>
+      <c r="E47" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="G47" s="7" t="s">
         <v>1</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I47" s="21"/>
       <c r="J47" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K47" s="9"/>
+      <c r="K47" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="M47" s="7" t="s">
         <v>1</v>
       </c>
       <c r="N47" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O47" s="21"/>
       <c r="P47" s="8" t="s">
         <v>4</v>
       </c>
       <c r="Q47" s="9" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
@@ -4237,33 +4466,45 @@
       <c r="B49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="6"/>
+      <c r="C49" s="6">
+        <v>2.2264869999999999E-2</v>
+      </c>
       <c r="D49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="11"/>
+      <c r="E49" s="11">
+        <v>0</v>
+      </c>
       <c r="G49" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I49" s="6"/>
+      <c r="I49" s="6">
+        <v>0.1083686</v>
+      </c>
       <c r="J49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K49" s="11"/>
+      <c r="K49" s="11">
+        <v>8.6866300000000007E-3</v>
+      </c>
       <c r="M49" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O49" s="6"/>
+      <c r="O49" s="6">
+        <v>3.0193089999999999E-2</v>
+      </c>
       <c r="P49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q49" s="11"/>
+      <c r="Q49" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
@@ -4272,33 +4513,45 @@
       <c r="B50" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="5"/>
+      <c r="C50" s="5">
+        <v>2.75</v>
+      </c>
       <c r="D50" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="12"/>
+      <c r="E50" s="12">
+        <v>37.81</v>
+      </c>
       <c r="G50" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I50" s="5"/>
+      <c r="I50" s="5">
+        <v>4.3499999999999996</v>
+      </c>
       <c r="J50" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K50" s="12"/>
+      <c r="K50" s="12">
+        <v>55.64</v>
+      </c>
       <c r="M50" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O50" s="5"/>
+      <c r="O50" s="5">
+        <v>12.71</v>
+      </c>
       <c r="P50" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q50" s="12"/>
+      <c r="Q50" s="12">
+        <v>181.76</v>
+      </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
@@ -4307,33 +4560,45 @@
       <c r="B51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="6"/>
+      <c r="C51" s="6">
+        <v>50</v>
+      </c>
       <c r="D51" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="11"/>
+      <c r="E51" s="11">
+        <v>50</v>
+      </c>
       <c r="G51" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="6"/>
+      <c r="I51" s="6">
+        <v>50</v>
+      </c>
       <c r="J51" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K51" s="11"/>
+      <c r="K51" s="11">
+        <v>70</v>
+      </c>
       <c r="M51" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O51" s="6"/>
+      <c r="O51" s="6">
+        <v>30</v>
+      </c>
       <c r="P51" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q51" s="11"/>
+      <c r="Q51" s="11">
+        <v>40</v>
+      </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="18" t="s">
@@ -4365,22 +4630,30 @@
       <c r="B53" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="6"/>
+      <c r="C53" s="6">
+        <v>2.2264869999999999E-2</v>
+      </c>
       <c r="D53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="11"/>
+      <c r="E53" s="11">
+        <v>0</v>
+      </c>
       <c r="G53" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="6"/>
+      <c r="I53" s="6">
+        <v>0.1083686</v>
+      </c>
       <c r="J53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K53" s="11"/>
+      <c r="K53" s="11">
+        <v>8.6866300000000007E-3</v>
+      </c>
       <c r="M53" s="10" t="s">
         <v>7</v>
       </c>
@@ -4404,22 +4677,30 @@
       <c r="B54" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="5"/>
+      <c r="C54" s="5">
+        <v>3.71</v>
+      </c>
       <c r="D54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="12"/>
+      <c r="E54" s="12">
+        <v>37.11</v>
+      </c>
       <c r="G54" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I54" s="5"/>
+      <c r="I54" s="5">
+        <v>3.05</v>
+      </c>
       <c r="J54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K54" s="12"/>
+      <c r="K54" s="12">
+        <v>33.39</v>
+      </c>
       <c r="M54" s="10" t="s">
         <v>27</v>
       </c>
@@ -4443,35 +4724,43 @@
       <c r="B55" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="5"/>
+      <c r="C55" s="27">
+        <v>40</v>
+      </c>
       <c r="D55" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="12"/>
+      <c r="E55" s="26">
+        <v>70</v>
+      </c>
       <c r="G55" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="5"/>
+      <c r="I55" s="27">
+        <v>40</v>
+      </c>
       <c r="J55" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K55" s="12"/>
+      <c r="K55" s="12">
+        <v>70</v>
+      </c>
       <c r="M55" s="13" t="s">
         <v>12</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O55" s="5">
+      <c r="O55" s="27">
         <v>40</v>
       </c>
       <c r="P55" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q55" s="12">
+      <c r="Q55" s="26">
         <v>70</v>
       </c>
     </row>
@@ -4605,7 +4894,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -4624,7 +4913,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="8" t="s">
@@ -4637,7 +4926,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="21"/>
       <c r="J3" s="8" t="s">
@@ -4648,7 +4937,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O3" s="21"/>
       <c r="P3" s="8" t="s">
@@ -4858,7 +5147,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -4981,7 +5270,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="8" t="s">
@@ -4992,7 +5281,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="8" t="s">
@@ -5003,7 +5292,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="8" t="s">
@@ -5320,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="8" t="s">
@@ -5331,7 +5620,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="8" t="s">
@@ -5342,7 +5631,7 @@
         <v>1</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O25" s="21"/>
       <c r="P25" s="8" t="s">
@@ -5659,7 +5948,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="8" t="s">
@@ -5670,7 +5959,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I36" s="21"/>
       <c r="J36" s="8" t="s">
@@ -5681,7 +5970,7 @@
         <v>1</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O36" s="21"/>
       <c r="P36" s="8" t="s">
@@ -5998,7 +6287,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="8" t="s">
@@ -6009,7 +6298,7 @@
         <v>1</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I47" s="21"/>
       <c r="J47" s="8" t="s">

</xml_diff>

<commit_message>
Updated TestResults.xlxs and added Argo Test Result Files
</commit_message>
<xml_diff>
--- a/RecreationExperiment/Test Results/TestResults.xlsx
+++ b/RecreationExperiment/Test Results/TestResults.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="64">
   <si>
     <t>ArgoUML</t>
   </si>
@@ -611,6 +611,18 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -618,18 +630,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -941,7 +941,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25:I25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,19 +973,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
@@ -1038,27 +1038,27 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="G4" s="23" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="G4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
-      <c r="M4" s="23" t="s">
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
+      <c r="M4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="25"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -1202,27 +1202,27 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="G8" s="23" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="G8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
-      <c r="M8" s="23" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+      <c r="M8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="25"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -1461,27 +1461,27 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="G15" s="23" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="G15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
-      <c r="M15" s="23" t="s">
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
+      <c r="M15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="25"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="29"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
@@ -1625,27 +1625,27 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="G19" s="23" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="G19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="25"/>
-      <c r="M19" s="23" t="s">
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
+      <c r="M19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="25"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="29"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
@@ -1860,7 +1860,9 @@
       <c r="J25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="9"/>
+      <c r="K25" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M25" s="7" t="s">
         <v>1</v>
       </c>
@@ -1876,27 +1878,27 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
-      <c r="G26" s="23" t="s">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="G26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25"/>
-      <c r="M26" s="23" t="s">
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="29"/>
+      <c r="M26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="25"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="29"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -2028,27 +2030,27 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25"/>
-      <c r="G30" s="23" t="s">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+      <c r="G30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="25"/>
-      <c r="M30" s="23" t="s">
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="29"/>
+      <c r="M30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="25"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="29"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
@@ -2251,7 +2253,9 @@
       <c r="J36" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K36" s="9"/>
+      <c r="K36" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M36" s="7" t="s">
         <v>1</v>
       </c>
@@ -2267,27 +2271,27 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
-      <c r="G37" s="23" t="s">
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
+      <c r="G37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="25"/>
-      <c r="M37" s="23" t="s">
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="29"/>
+      <c r="M37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="25"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="29"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
@@ -2311,11 +2315,15 @@
       <c r="H38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="6"/>
+      <c r="I38" s="6">
+        <v>2.263575E-2</v>
+      </c>
       <c r="J38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K38" s="11"/>
+      <c r="K38" s="11">
+        <v>1.9903400000000002E-2</v>
+      </c>
       <c r="M38" s="10" t="s">
         <v>7</v>
       </c>
@@ -2354,11 +2362,15 @@
       <c r="H39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I39" s="5"/>
+      <c r="I39" s="5">
+        <v>39.53</v>
+      </c>
       <c r="J39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K39" s="12"/>
+      <c r="K39" s="12">
+        <v>420.51</v>
+      </c>
       <c r="M39" s="10" t="s">
         <v>27</v>
       </c>
@@ -2397,11 +2409,15 @@
       <c r="H40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="6"/>
+      <c r="I40" s="6">
+        <v>55</v>
+      </c>
       <c r="J40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="11"/>
+      <c r="K40" s="11">
+        <v>73</v>
+      </c>
       <c r="M40" s="13" t="s">
         <v>12</v>
       </c>
@@ -2419,27 +2435,27 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
-      <c r="G41" s="23" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29"/>
+      <c r="G41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="25"/>
-      <c r="M41" s="23" t="s">
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="29"/>
+      <c r="M41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="25"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="29"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
@@ -2463,11 +2479,15 @@
       <c r="H42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="6"/>
+      <c r="I42" s="6">
+        <v>2.263575E-2</v>
+      </c>
       <c r="J42" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K42" s="11"/>
+      <c r="K42" s="11">
+        <v>1.9903400000000002E-2</v>
+      </c>
       <c r="M42" s="10" t="s">
         <v>7</v>
       </c>
@@ -2506,11 +2526,15 @@
       <c r="H43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="5"/>
+      <c r="I43" s="5">
+        <v>39.090000000000003</v>
+      </c>
       <c r="J43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K43" s="12"/>
+      <c r="K43" s="12">
+        <v>311.36</v>
+      </c>
       <c r="M43" s="10" t="s">
         <v>27</v>
       </c>
@@ -2549,11 +2573,15 @@
       <c r="H44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I44" s="5"/>
+      <c r="I44" s="5">
+        <v>68</v>
+      </c>
       <c r="J44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K44" s="12"/>
+      <c r="K44" s="12">
+        <v>79</v>
+      </c>
       <c r="M44" s="13" t="s">
         <v>12</v>
       </c>
@@ -2647,20 +2675,20 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
-      <c r="G48" s="23" t="s">
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="29"/>
+      <c r="G48" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="25"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="29"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -2759,20 +2787,20 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="25"/>
-      <c r="G52" s="23" t="s">
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29"/>
+      <c r="G52" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="25"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="29"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
@@ -2906,6 +2934,33 @@
     <row r="80" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="M41:Q41"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="G48:K48"/>
+    <mergeCell ref="G52:K52"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="M26:Q26"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="M37:Q37"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="M4:Q4"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A15:E15"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="A37:E37"/>
@@ -2922,33 +2977,6 @@
     <mergeCell ref="G41:K41"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A8:E8"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="M26:Q26"/>
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="M37:Q37"/>
-    <mergeCell ref="M41:Q41"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="G48:K48"/>
-    <mergeCell ref="G52:K52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3046,27 +3074,27 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="G4" s="23" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="G4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
-      <c r="M4" s="23" t="s">
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
+      <c r="M4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="25"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -3210,27 +3238,27 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="G8" s="23" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="G8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
-      <c r="M8" s="23" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+      <c r="M8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="25"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -3469,27 +3497,27 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="G15" s="23" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="G15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
-      <c r="M15" s="23" t="s">
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
+      <c r="M15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="25"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="29"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
@@ -3633,27 +3661,27 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="G19" s="23" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="G19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="25"/>
-      <c r="M19" s="23" t="s">
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
+      <c r="M19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="25"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="29"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
@@ -3886,27 +3914,27 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
-      <c r="G26" s="23" t="s">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="G26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25"/>
-      <c r="M26" s="23" t="s">
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="29"/>
+      <c r="M26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="25"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="29"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -4050,27 +4078,27 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25"/>
-      <c r="G30" s="23" t="s">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+      <c r="G30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="25"/>
-      <c r="M30" s="23" t="s">
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="29"/>
+      <c r="M30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="25"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="29"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
@@ -4303,27 +4331,27 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
-      <c r="G37" s="23" t="s">
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
+      <c r="G37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="25"/>
-      <c r="M37" s="23" t="s">
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="29"/>
+      <c r="M37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="25"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="29"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
@@ -4467,27 +4495,27 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
-      <c r="G41" s="23" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29"/>
+      <c r="G41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="25"/>
-      <c r="M41" s="23" t="s">
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="29"/>
+      <c r="M41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="25"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="29"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
@@ -4677,7 +4705,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:17" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>1</v>
@@ -4720,27 +4748,27 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
-      <c r="G48" s="23" t="s">
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="29"/>
+      <c r="G48" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="25"/>
-      <c r="M48" s="23" t="s">
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="29"/>
+      <c r="M48" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N48" s="24"/>
-      <c r="O48" s="24"/>
-      <c r="P48" s="24"/>
-      <c r="Q48" s="25"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="28"/>
+      <c r="P48" s="28"/>
+      <c r="Q48" s="29"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -4884,27 +4912,27 @@
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="25"/>
-      <c r="G52" s="23" t="s">
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29"/>
+      <c r="G52" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="25"/>
-      <c r="M52" s="23" t="s">
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="29"/>
+      <c r="M52" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N52" s="24"/>
-      <c r="O52" s="24"/>
-      <c r="P52" s="24"/>
-      <c r="Q52" s="25"/>
+      <c r="N52" s="28"/>
+      <c r="O52" s="28"/>
+      <c r="P52" s="28"/>
+      <c r="Q52" s="29"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
@@ -5096,36 +5124,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="M26:Q26"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="N36:O36"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="N47:O47"/>
     <mergeCell ref="M48:Q48"/>
@@ -5142,6 +5140,36 @@
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="G41:K41"/>
     <mergeCell ref="M41:Q41"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="M26:Q26"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="M4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5229,27 +5257,27 @@
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="G4" s="23" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="G4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
-      <c r="M4" s="23" t="s">
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
+      <c r="M4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="25"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
     </row>
     <row r="5" spans="1:17" ht="26.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -5361,27 +5389,27 @@
       <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="G8" s="23" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="G8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
-      <c r="M8" s="23" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+      <c r="M8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="25"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
     </row>
     <row r="9" spans="1:17" ht="26.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
@@ -5584,27 +5612,27 @@
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="G15" s="23" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="G15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
-      <c r="M15" s="23" t="s">
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
+      <c r="M15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="25"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="29"/>
     </row>
     <row r="16" spans="1:17" ht="26.1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
@@ -5712,27 +5740,27 @@
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="G19" s="23" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="G19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="25"/>
-      <c r="M19" s="23" t="s">
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
+      <c r="M19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="25"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="29"/>
     </row>
     <row r="20" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
@@ -5923,27 +5951,27 @@
       <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
-      <c r="G26" s="23" t="s">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="G26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25"/>
-      <c r="M26" s="23" t="s">
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="29"/>
+      <c r="M26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="25"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="29"/>
     </row>
     <row r="27" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
@@ -6051,27 +6079,27 @@
       <c r="Q29" s="11"/>
     </row>
     <row r="30" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25"/>
-      <c r="G30" s="23" t="s">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+      <c r="G30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="25"/>
-      <c r="M30" s="23" t="s">
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="29"/>
+      <c r="M30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="25"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="29"/>
     </row>
     <row r="31" spans="1:17" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
@@ -6262,27 +6290,27 @@
       <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
-      <c r="G37" s="23" t="s">
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
+      <c r="G37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="25"/>
-      <c r="M37" s="23" t="s">
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="29"/>
+      <c r="M37" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="25"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="29"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
@@ -6390,27 +6418,27 @@
       <c r="Q40" s="11"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
-      <c r="G41" s="23" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29"/>
+      <c r="G41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="25"/>
-      <c r="M41" s="23" t="s">
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="29"/>
+      <c r="M41" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="25"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="29"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
@@ -6590,20 +6618,20 @@
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
-      <c r="G48" s="23" t="s">
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="29"/>
+      <c r="G48" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="25"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="29"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -6678,20 +6706,20 @@
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="25"/>
-      <c r="G52" s="23" t="s">
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29"/>
+      <c r="G52" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="25"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="29"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
@@ -6799,36 +6827,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="M26:Q26"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="M37:Q37"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="G41:K41"/>
-    <mergeCell ref="M41:Q41"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="N36:O36"/>
     <mergeCell ref="A52:E52"/>
     <mergeCell ref="G52:K52"/>
     <mergeCell ref="A1:K1"/>
@@ -6842,6 +6840,36 @@
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="G8:K8"/>
+    <mergeCell ref="M37:Q37"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="G41:K41"/>
+    <mergeCell ref="M41:Q41"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="M26:Q26"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="M4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>